<commit_message>
Incluído el estado 'Lobby'
</commit_message>
<xml_diff>
--- a/docs/GS-CR-v1.0.xlsx
+++ b/docs/GS-CR-v1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Borjis\Dropbox\Videojuegos\Diseño\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Borjis\BitBucket\galactic-strike-socket-io\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -245,9 +245,6 @@
     <t>Sprite estático para objetos</t>
   </si>
   <si>
-    <t>Movimiendo básico del personaje</t>
-  </si>
-  <si>
     <t>Tilesheets</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Movimiento básico del personaje</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -558,7 +558,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
@@ -570,8 +570,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1045,7 +1045,7 @@
   <dimension ref="B1:K154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,17 +1074,17 @@
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>84</v>
+      <c r="J3" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -1092,17 +1092,17 @@
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
-      <c r="H4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>85</v>
+      <c r="H4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1150,7 +1150,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
     </row>
     <row r="10" spans="2:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1168,14 +1168,14 @@
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="45" x14ac:dyDescent="0.25">
@@ -1184,7 +1184,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="45" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1282,14 +1282,14 @@
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -1359,7 +1359,7 @@
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="17" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1396,14 +1396,14 @@
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
         <v>37</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>39</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -1475,7 +1475,7 @@
       <c r="C50" s="6"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="17" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="6" t="s">
@@ -1517,7 +1517,7 @@
       <c r="C55" s="6"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="17" t="s">
         <v>47</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -1549,7 +1549,7 @@
       <c r="C60" s="6"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="17" t="s">
         <v>51</v>
       </c>
       <c r="C61" s="6" t="s">
@@ -1581,7 +1581,7 @@
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="17" t="s">
         <v>54</v>
       </c>
       <c r="C66" s="6" t="s">
@@ -1654,7 +1654,7 @@
       <c r="C75" s="6"/>
     </row>
     <row r="76" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="17" t="s">
         <v>61</v>
       </c>
       <c r="C76" s="6" t="s">
@@ -1725,14 +1725,14 @@
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="17" t="s">
         <v>69</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1741,7 +1741,7 @@
         <v>71</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
     <row r="89" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B89" s="15"/>
       <c r="C89" s="10" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>9</v>
@@ -1765,7 +1765,7 @@
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="15"/>
       <c r="C90" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>9</v>
@@ -1774,7 +1774,7 @@
     <row r="91" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="15"/>
       <c r="C91" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>9</v>
@@ -1786,10 +1786,10 @@
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>9</v>
@@ -1803,7 +1803,7 @@
     <row r="95" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B95" s="19"/>
       <c r="C95" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>9</v>
@@ -1999,12 +1999,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B101:B105"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="B66:B75"/>
-    <mergeCell ref="B76:B85"/>
-    <mergeCell ref="B86:B92"/>
-    <mergeCell ref="B93:B100"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B21:B25"/>
@@ -2013,6 +2007,12 @@
     <mergeCell ref="B41:B50"/>
     <mergeCell ref="B36:B40"/>
     <mergeCell ref="B51:B55"/>
+    <mergeCell ref="B101:B105"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B66:B75"/>
+    <mergeCell ref="B76:B85"/>
+    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="B93:B100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Menos firerate + CD compartido + llamadas a socket.emit('attack') optimizadas
</commit_message>
<xml_diff>
--- a/docs/GS-CR-v1.0.xlsx
+++ b/docs/GS-CR-v1.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
   <si>
     <t>Prototipo (P2)</t>
   </si>
@@ -552,13 +552,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
@@ -568,9 +571,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,18 +1121,18 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1141,16 +1141,16 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
     </row>
     <row r="10" spans="2:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="21"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1168,7 +1168,7 @@
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1179,25 +1179,25 @@
       </c>
     </row>
     <row r="12" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1206,7 +1206,7 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1224,7 +1224,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1242,7 +1242,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1261,57 +1261,57 @@
       </c>
     </row>
     <row r="22" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1320,7 +1320,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="15"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="7" t="s">
         <v>30</v>
       </c>
@@ -1329,7 +1329,7 @@
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="15"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="6" t="s">
         <v>28</v>
       </c>
@@ -1338,7 +1338,7 @@
       </c>
     </row>
     <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="15"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1347,19 +1347,19 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="15"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="15"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="16"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1370,7 +1370,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="15"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="2" t="s">
         <v>33</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="15"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="2" t="s">
         <v>34</v>
       </c>
@@ -1388,15 +1388,15 @@
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="15"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="16"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1407,7 +1407,7 @@
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="15"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="7" t="s">
         <v>41</v>
       </c>
@@ -1416,7 +1416,7 @@
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="15"/>
+      <c r="B43" s="16"/>
       <c r="C43" s="6" t="s">
         <v>37</v>
       </c>
@@ -1425,16 +1425,16 @@
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="15"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="15"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="6" t="s">
         <v>38</v>
       </c>
@@ -1443,16 +1443,16 @@
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="15"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="15"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="6" t="s">
         <v>42</v>
       </c>
@@ -1461,21 +1461,21 @@
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="15"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="6"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="15"/>
+      <c r="B49" s="16"/>
       <c r="C49" s="6"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="16"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="6"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="15" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="6" t="s">
@@ -1486,7 +1486,7 @@
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="15"/>
+      <c r="B52" s="16"/>
       <c r="C52" s="6" t="s">
         <v>45</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="15"/>
+      <c r="B53" s="16"/>
       <c r="C53" s="6" t="s">
         <v>49</v>
       </c>
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="15"/>
+      <c r="B54" s="16"/>
       <c r="C54" s="6" t="s">
         <v>50</v>
       </c>
@@ -1513,11 +1513,11 @@
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="16"/>
+      <c r="B55" s="17"/>
       <c r="C55" s="6"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -1528,7 +1528,7 @@
       </c>
     </row>
     <row r="57" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B57" s="15"/>
+      <c r="B57" s="16"/>
       <c r="C57" s="6" t="s">
         <v>48</v>
       </c>
@@ -1537,19 +1537,19 @@
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="15"/>
+      <c r="B58" s="16"/>
       <c r="C58" s="6"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="15"/>
+      <c r="B59" s="16"/>
       <c r="C59" s="6"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="16"/>
+      <c r="B60" s="17"/>
       <c r="C60" s="6"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="15" t="s">
         <v>51</v>
       </c>
       <c r="C61" s="6" t="s">
@@ -1560,7 +1560,7 @@
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="15"/>
+      <c r="B62" s="16"/>
       <c r="C62" s="6" t="s">
         <v>53</v>
       </c>
@@ -1569,39 +1569,39 @@
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="15"/>
+      <c r="B63" s="16"/>
       <c r="C63" s="6"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="15"/>
+      <c r="B64" s="16"/>
       <c r="C64" s="6"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="16"/>
+      <c r="B65" s="17"/>
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="15" t="s">
         <v>54</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B67" s="15"/>
+      <c r="B67" s="16"/>
       <c r="C67" s="6" t="s">
         <v>56</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B68" s="15"/>
+      <c r="B68" s="16"/>
       <c r="C68" s="6" t="s">
         <v>57</v>
       </c>
@@ -1610,7 +1610,7 @@
       </c>
     </row>
     <row r="69" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B69" s="15"/>
+      <c r="B69" s="16"/>
       <c r="C69" s="6" t="s">
         <v>58</v>
       </c>
@@ -1619,7 +1619,7 @@
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="15"/>
+      <c r="B70" s="16"/>
       <c r="C70" s="6" t="s">
         <v>59</v>
       </c>
@@ -1629,7 +1629,7 @@
       <c r="H70" s="9"/>
     </row>
     <row r="71" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B71" s="15"/>
+      <c r="B71" s="16"/>
       <c r="C71" s="6" t="s">
         <v>60</v>
       </c>
@@ -1638,43 +1638,43 @@
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="15"/>
+      <c r="B72" s="16"/>
       <c r="C72" s="6"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="15"/>
+      <c r="B73" s="16"/>
       <c r="C73" s="6"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="15"/>
+      <c r="B74" s="16"/>
       <c r="C74" s="6"/>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="16"/>
+      <c r="B75" s="17"/>
       <c r="C75" s="6"/>
     </row>
     <row r="76" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>62</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="15"/>
+      <c r="B77" s="16"/>
       <c r="C77" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="15"/>
+      <c r="B78" s="16"/>
       <c r="C78" s="6" t="s">
         <v>64</v>
       </c>
@@ -1683,7 +1683,7 @@
       </c>
     </row>
     <row r="79" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B79" s="15"/>
+      <c r="B79" s="16"/>
       <c r="C79" s="6" t="s">
         <v>65</v>
       </c>
@@ -1692,40 +1692,43 @@
       </c>
     </row>
     <row r="80" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="15"/>
+      <c r="B80" s="16"/>
       <c r="C80" s="6" t="s">
         <v>66</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="15"/>
+      <c r="B81" s="16"/>
       <c r="C81" s="6" t="s">
         <v>67</v>
       </c>
+      <c r="D81" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="16" t="s">
         <v>68</v>
       </c>
       <c r="C82" s="6"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="15"/>
+      <c r="B83" s="16"/>
       <c r="C83" s="6"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="15"/>
+      <c r="B84" s="16"/>
       <c r="C84" s="6"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="16"/>
+      <c r="B85" s="17"/>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="15" t="s">
         <v>69</v>
       </c>
       <c r="C86" s="2" t="s">
@@ -1736,7 +1739,7 @@
       </c>
     </row>
     <row r="87" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B87" s="15"/>
+      <c r="B87" s="16"/>
       <c r="C87" s="2" t="s">
         <v>71</v>
       </c>
@@ -1745,7 +1748,7 @@
       </c>
     </row>
     <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B88" s="15"/>
+      <c r="B88" s="16"/>
       <c r="C88" s="2" t="s">
         <v>72</v>
       </c>
@@ -1754,7 +1757,7 @@
       </c>
     </row>
     <row r="89" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B89" s="15"/>
+      <c r="B89" s="16"/>
       <c r="C89" s="10" t="s">
         <v>85</v>
       </c>
@@ -1763,7 +1766,7 @@
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="15"/>
+      <c r="B90" s="16"/>
       <c r="C90" s="2" t="s">
         <v>73</v>
       </c>
@@ -1772,7 +1775,7 @@
       </c>
     </row>
     <row r="91" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B91" s="15"/>
+      <c r="B91" s="16"/>
       <c r="C91" s="2" t="s">
         <v>74</v>
       </c>
@@ -1781,27 +1784,27 @@
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="15"/>
+      <c r="B92" s="16"/>
       <c r="C92" s="6"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="19" t="s">
         <v>75</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="19"/>
+      <c r="B94" s="20"/>
       <c r="C94" s="6"/>
       <c r="E94" s="8"/>
     </row>
     <row r="95" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B95" s="19"/>
+      <c r="B95" s="20"/>
       <c r="C95" s="6" t="s">
         <v>77</v>
       </c>
@@ -1810,43 +1813,43 @@
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="19"/>
+      <c r="B96" s="20"/>
       <c r="C96" s="6"/>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="19"/>
+      <c r="B97" s="20"/>
       <c r="C97" s="6"/>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="19"/>
+      <c r="B98" s="20"/>
       <c r="C98" s="6"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="19"/>
+      <c r="B99" s="20"/>
       <c r="C99" s="6"/>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="20"/>
+      <c r="B100" s="21"/>
       <c r="C100" s="6"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="15"/>
+      <c r="B101" s="16"/>
       <c r="C101" s="6"/>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="15"/>
+      <c r="B102" s="16"/>
       <c r="C102" s="6"/>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="15"/>
+      <c r="B103" s="16"/>
       <c r="C103" s="6"/>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="15"/>
+      <c r="B104" s="16"/>
       <c r="C104" s="6"/>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="16"/>
+      <c r="B105" s="17"/>
       <c r="C105" s="6"/>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
@@ -1999,6 +2002,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B101:B105"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B66:B75"/>
+    <mergeCell ref="B76:B85"/>
+    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="B93:B100"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B21:B25"/>
@@ -2007,12 +2016,6 @@
     <mergeCell ref="B41:B50"/>
     <mergeCell ref="B36:B40"/>
     <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B101:B105"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="B66:B75"/>
-    <mergeCell ref="B76:B85"/>
-    <mergeCell ref="B86:B92"/>
-    <mergeCell ref="B93:B100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>